<commit_message>
Progress toward single line model assessment
</commit_message>
<xml_diff>
--- a/Import Scripts/voltageClamp/protocols.xlsx
+++ b/Import Scripts/voltageClamp/protocols.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\neuroml-db\Import Scripts\voltageClamp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="20120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="20115" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>Time</t>
   </si>
@@ -30,13 +35,7 @@
     <t>Na</t>
   </si>
   <si>
-    <t>Na-low</t>
-  </si>
-  <si>
     <t>Ih</t>
-  </si>
-  <si>
-    <t>Ih-low</t>
   </si>
   <si>
     <t>Na/Kv/KCa/Cav</t>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -107,12 +106,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -159,7 +164,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -168,6 +173,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -206,11 +212,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -253,22 +267,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,27 +294,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4F0C-4880-BFCC-21A0024C61A5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -311,7 +330,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Kv/KCa/Cav</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -326,22 +345,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -353,27 +372,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4F0C-4880-BFCC-21A0024C61A5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -428,14 +452,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -478,22 +502,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,27 +529,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9181-4558-B7CC-540E1C500349}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -536,7 +565,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Na-low</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -551,22 +580,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,27 +607,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9181-4558-B7CC-540E1C500349}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -653,14 +687,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -703,22 +737,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2100.0</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2100.0</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2130.0</c:v>
+                  <c:v>2130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -730,27 +764,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8419-48CF-A89E-4CE88B9D7019}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -761,7 +800,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ih-low</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -776,22 +815,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2100.0</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2100.0</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2130.0</c:v>
+                  <c:v>2130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -803,27 +842,32 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-150.0</c:v>
+                  <c:v>-150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-150.0</c:v>
+                  <c:v>-150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8419-48CF-A89E-4CE88B9D7019}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -878,14 +922,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -928,28 +972,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1600.0</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1600.0</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1650.0</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1650.0</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1750.0</c:v>
+                  <c:v>1750</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -961,44 +1005,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8928-4790-9231-1B75F771F8E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$25</c:f>
+              <c:f>Sheet1!$D$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Na/Kv/KCa/Cav low</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1013,28 +1062,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1600.0</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1600.0</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1650.0</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1650.0</c:v>
+                  <c:v>1650</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1750.0</c:v>
+                  <c:v>1750</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1046,33 +1095,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8928-4790-9231-1B75F771F8E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1127,14 +1181,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1177,28 +1231,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1100.0</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1100.0</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1400.0</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1400.0</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1500.0</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1210,33 +1264,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-150.0</c:v>
+                  <c:v>-150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-150.0</c:v>
+                  <c:v>-150</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-120.0</c:v>
+                  <c:v>-120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-120.0</c:v>
+                  <c:v>-120</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8918-4F43-8D65-84141ACE9135}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1247,7 +1306,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ih-low</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1262,28 +1321,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1100.0</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1100.0</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1400.0</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1400.0</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1500.0</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1295,33 +1354,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-120.0</c:v>
+                  <c:v>-120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-120.0</c:v>
+                  <c:v>-120</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8918-4F43-8D65-84141ACE9135}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1376,14 +1440,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1426,28 +1490,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1459,33 +1523,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-75A0-4781-981F-7CD3E62D6330}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1496,7 +1565,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Kv/KCa/Cav</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1511,28 +1580,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>700.0</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1544,33 +1613,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-100.0</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-100.0</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-75A0-4781-981F-7CD3E62D6330}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1625,14 +1699,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1675,28 +1749,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1708,33 +1782,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E48-4635-8B92-E3614A5BE4A8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1745,7 +1824,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Na-low</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1760,28 +1839,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1793,33 +1872,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-100.0</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-100.0</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-80.0</c:v>
+                  <c:v>-80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E48-4635-8B92-E3614A5BE4A8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1874,14 +1958,14 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1924,28 +2008,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1600.0</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1600.0</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2100.0</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2100.0</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2600.0</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1957,33 +2041,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-140.0</c:v>
+                  <c:v>-140</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-140.0</c:v>
+                  <c:v>-140</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-34E2-4BA5-B83A-6F53AD2B6696}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1994,7 +2083,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ih-low</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2009,28 +2098,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1600.0</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1600.0</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2100.0</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2100.0</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2600.0</c:v>
+                  <c:v>2600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2042,33 +2131,38 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-140.0</c:v>
+                  <c:v>-140</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-140.0</c:v>
+                  <c:v>-140</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-110.0</c:v>
+                  <c:v>-110</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-110.0</c:v>
+                  <c:v>-110</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-34E2-4BA5-B83A-6F53AD2B6696}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2123,7 +2217,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2201,7 +2295,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>698500</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -2265,7 +2359,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>698500</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -2361,7 +2455,7 @@
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -2710,22 +2804,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -2734,20 +2828,20 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
+      <c r="F1" s="4">
+        <v>2</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="I1" s="4">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2776,13 +2870,13 @@
         <f>H2</f>
         <v>-40</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100</v>
       </c>
@@ -2816,55 +2910,56 @@
         <f>H3</f>
         <v>-40</v>
       </c>
-      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3</f>
         <v>100</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>70</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>-80</v>
       </c>
       <c r="D4" s="1">
         <f>D3</f>
         <v>20</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>70</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>-80</v>
       </c>
       <c r="G4" s="1">
         <f>G3</f>
         <v>100</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>-150</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+500</f>
         <v>600</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <f>B4</f>
         <v>70</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <f>C4</f>
         <v>-80</v>
       </c>
@@ -2872,11 +2967,11 @@
         <f>D4+50</f>
         <v>70</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <f>E4</f>
         <v>70</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <f>F4</f>
         <v>-80</v>
       </c>
@@ -2884,16 +2979,17 @@
         <f>G4+2000</f>
         <v>2100</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <f>H4</f>
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <f>I4</f>
         <v>-150</v>
       </c>
+      <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5</f>
         <v>600</v>
@@ -2930,11 +3026,11 @@
         <f>H6</f>
         <v>-40</v>
       </c>
-      <c r="K6" t="s">
-        <v>10</v>
+      <c r="L6" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6+100</f>
         <v>700</v>
@@ -2971,32 +3067,31 @@
         <f>H7</f>
         <v>-40</v>
       </c>
-      <c r="K7" t="s">
-        <v>11</v>
+      <c r="L7" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="str">
-        <f>B25&amp;" low"</f>
-        <v>Na/Kv/KCa/Cav low</v>
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3005,6 +3100,10 @@
       </c>
       <c r="C26">
         <v>-80</v>
+      </c>
+      <c r="D26" t="b">
+        <f>C26=B26</f>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -3016,13 +3115,17 @@
         <f>H26</f>
         <v>-40</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K26" s="2"/>
+      <c r="J26" t="b">
+        <f t="shared" ref="J26:J33" si="0">I26=H26</f>
+        <v>1</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>100</v>
       </c>
@@ -3033,6 +3136,10 @@
       <c r="C27">
         <f>C26</f>
         <v>-80</v>
+      </c>
+      <c r="D27" t="b">
+        <f t="shared" ref="D27:D33" si="1">C27=B27</f>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>100</v>
@@ -3045,62 +3152,82 @@
         <f>I26</f>
         <v>-40</v>
       </c>
-      <c r="J27" s="2"/>
+      <c r="J27" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A27</f>
         <v>100</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="4">
         <v>70</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <v>-40</v>
+      </c>
+      <c r="D28" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G28">
         <f>G27</f>
         <v>100</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="4">
         <v>-150</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="4">
         <v>-40</v>
       </c>
-      <c r="J28" s="2"/>
+      <c r="J28" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>A28+1500</f>
         <v>1600</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <f>B28</f>
         <v>70</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4">
         <f>C28</f>
         <v>-40</v>
+      </c>
+      <c r="D29" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G29">
         <f>G28+1000</f>
         <v>1100</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="4">
         <f>H28</f>
         <v>-150</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="4">
         <f>I28</f>
         <v>-40</v>
       </c>
+      <c r="J29" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>A29</f>
         <v>1600</v>
@@ -3112,6 +3239,10 @@
         <f>B30</f>
         <v>30</v>
       </c>
+      <c r="D30" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="G30">
         <f>G29</f>
         <v>1100</v>
@@ -3123,8 +3254,12 @@
         <f>H30</f>
         <v>-120</v>
       </c>
+      <c r="J30" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>A30+50</f>
         <v>1650</v>
@@ -3137,6 +3272,10 @@
         <f>B30</f>
         <v>30</v>
       </c>
+      <c r="D31" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="G31">
         <f>G30+300</f>
         <v>1400</v>
@@ -3149,8 +3288,12 @@
         <f>H30</f>
         <v>-120</v>
       </c>
+      <c r="J31" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>A31</f>
         <v>1650</v>
@@ -3162,6 +3305,10 @@
         <f>B32</f>
         <v>-80</v>
       </c>
+      <c r="D32" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="G32">
         <f>G31</f>
         <v>1400</v>
@@ -3174,8 +3321,12 @@
         <f>H32</f>
         <v>-40</v>
       </c>
+      <c r="J32" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>A31+100</f>
         <v>1750</v>
@@ -3188,6 +3339,10 @@
         <f>B32</f>
         <v>-80</v>
       </c>
+      <c r="D33" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="G33">
         <f>G31+100</f>
         <v>1500</v>
@@ -3200,16 +3355,20 @@
         <f>H33</f>
         <v>-40</v>
       </c>
+      <c r="J33" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>0</v>
       </c>
       <c r="B51" t="s">
         <v>1</v>
       </c>
-      <c r="C51" t="s">
-        <v>1</v>
+      <c r="C51">
+        <v>6</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>0</v>
@@ -3217,25 +3376,25 @@
       <c r="E51" t="s">
         <v>2</v>
       </c>
-      <c r="F51" t="s">
-        <v>3</v>
+      <c r="F51">
+        <v>7</v>
       </c>
       <c r="G51" t="s">
         <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>4</v>
-      </c>
-      <c r="I51" t="s">
-        <v>5</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K51" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I51">
+        <v>8</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0</v>
       </c>
@@ -3264,11 +3423,11 @@
         <f>H52</f>
         <v>-40</v>
       </c>
-      <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>100</v>
       </c>
@@ -3302,11 +3461,11 @@
         <f>I52</f>
         <v>-40</v>
       </c>
-      <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <f>A53</f>
         <v>100</v>
@@ -3339,7 +3498,7 @@
         <v>-140</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <f>A54+300</f>
         <v>400</v>
@@ -3375,77 +3534,77 @@
         <v>-140</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
-      <c r="A56">
+    <row r="56" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
         <f>A55</f>
         <v>400</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="4">
         <v>40</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="4">
         <v>-100</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="4">
         <f>D55</f>
         <v>30</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="4">
         <v>40</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="4">
         <v>-100</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="4">
         <f>G55</f>
         <v>1600</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="4">
         <v>0</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="4">
         <v>-110</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
-      <c r="A57">
+    <row r="57" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
         <f>A56+200</f>
         <v>600</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="4">
         <f>B56</f>
         <v>40</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="4">
         <f>C56</f>
         <v>-100</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="4">
         <f>D56+30</f>
         <v>60</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="4">
         <f>E56</f>
         <v>40</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="4">
         <f>F56</f>
         <v>-100</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="4">
         <f>G56+500</f>
         <v>2100</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="4">
         <f>H56</f>
         <v>0</v>
       </c>
-      <c r="I57">
+      <c r="I57" s="4">
         <f>I56</f>
         <v>-110</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <f>A57</f>
         <v>600</v>
@@ -3480,7 +3639,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <f>A57+100</f>
         <v>700</v>
@@ -3518,9 +3677,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="J2:L4"/>
-    <mergeCell ref="J26:L28"/>
-    <mergeCell ref="J51:L53"/>
+    <mergeCell ref="K2:M4"/>
+    <mergeCell ref="K26:M28"/>
+    <mergeCell ref="K51:M53"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>